<commit_message>
Cleaned up code to different files
created functions to clean up code + make it more modular for future GUI implementation
</commit_message>
<xml_diff>
--- a/Results_2018.xlsx
+++ b/Results_2018.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="All Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Successful Assignments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -5201,7 +5201,7 @@
         <v>681</v>
       </c>
       <c r="H94" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="I94" t="s">
         <v>695</v>
@@ -5343,10 +5343,10 @@
         <v>594</v>
       </c>
       <c r="G99" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="H99" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="I99" t="s">
         <v>691</v>
@@ -5372,10 +5372,10 @@
         <v>595</v>
       </c>
       <c r="G100" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H100" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="I100" t="s">
         <v>701</v>
@@ -5433,7 +5433,7 @@
         <v>680</v>
       </c>
       <c r="H102" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="I102" t="s">
         <v>690</v>
@@ -5462,7 +5462,7 @@
         <v>680</v>
       </c>
       <c r="H103" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="I103" t="s">
         <v>692</v>
@@ -5578,7 +5578,7 @@
         <v>688</v>
       </c>
       <c r="H107" t="s">
-        <v>684</v>
+        <v>674</v>
       </c>
       <c r="I107" t="s">
         <v>691</v>
@@ -5604,10 +5604,10 @@
         <v>603</v>
       </c>
       <c r="G108" t="s">
+        <v>687</v>
+      </c>
+      <c r="H108" t="s">
         <v>684</v>
-      </c>
-      <c r="H108" t="s">
-        <v>687</v>
       </c>
       <c r="I108" t="s">
         <v>691</v>
@@ -5691,10 +5691,10 @@
         <v>606</v>
       </c>
       <c r="G111" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H111" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="I111" t="s">
         <v>691</v>
@@ -5720,10 +5720,10 @@
         <v>607</v>
       </c>
       <c r="G112" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H112" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
       <c r="I112" t="s">
         <v>691</v>
@@ -5749,10 +5749,10 @@
         <v>608</v>
       </c>
       <c r="G113" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="H113" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="I113" t="s">
         <v>691</v>
@@ -5778,10 +5778,10 @@
         <v>609</v>
       </c>
       <c r="G114" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="H114" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
       <c r="I114" t="s">
         <v>690</v>
@@ -5807,10 +5807,10 @@
         <v>610</v>
       </c>
       <c r="G115" t="s">
+        <v>673</v>
+      </c>
+      <c r="H115" t="s">
         <v>688</v>
-      </c>
-      <c r="H115" t="s">
-        <v>673</v>
       </c>
       <c r="I115" t="s">
         <v>691</v>
@@ -5836,10 +5836,10 @@
         <v>611</v>
       </c>
       <c r="G116" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="H116" t="s">
-        <v>688</v>
+        <v>676</v>
       </c>
       <c r="I116" t="s">
         <v>691</v>
@@ -5865,10 +5865,10 @@
         <v>612</v>
       </c>
       <c r="G117" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H117" t="s">
-        <v>687</v>
+        <v>678</v>
       </c>
       <c r="I117" t="s">
         <v>690</v>
@@ -5894,10 +5894,10 @@
         <v>613</v>
       </c>
       <c r="G118" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="H118" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="I118" t="s">
         <v>691</v>
@@ -5923,10 +5923,10 @@
         <v>614</v>
       </c>
       <c r="G119" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="H119" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="I119" t="s">
         <v>692</v>
@@ -5955,7 +5955,7 @@
         <v>686</v>
       </c>
       <c r="H120" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="I120" t="s">
         <v>691</v>
@@ -6010,10 +6010,10 @@
         <v>617</v>
       </c>
       <c r="G122" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="H122" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="I122" t="s">
         <v>691</v>
@@ -6097,10 +6097,10 @@
         <v>620</v>
       </c>
       <c r="G125" t="s">
-        <v>689</v>
+        <v>673</v>
       </c>
       <c r="H125" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="I125" t="s">
         <v>691</v>
@@ -6300,10 +6300,10 @@
         <v>627</v>
       </c>
       <c r="G132" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="H132" t="s">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="I132" t="s">
         <v>691</v>
@@ -6619,10 +6619,10 @@
         <v>638</v>
       </c>
       <c r="G143" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="H143" t="s">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="I143" t="s">
         <v>691</v>
@@ -6677,10 +6677,10 @@
         <v>640</v>
       </c>
       <c r="G145" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="H145" t="s">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="I145" t="s">
         <v>691</v>
@@ -6996,10 +6996,10 @@
         <v>651</v>
       </c>
       <c r="G156" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="H156" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="I156" t="s">
         <v>691</v>
@@ -7112,10 +7112,10 @@
         <v>655</v>
       </c>
       <c r="G160" t="s">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="H160" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="I160" t="s">
         <v>691</v>
@@ -7460,10 +7460,10 @@
         <v>667</v>
       </c>
       <c r="G172" t="s">
-        <v>673</v>
+        <v>689</v>
       </c>
       <c r="H172" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="I172" t="s">
         <v>691</v>
@@ -10344,7 +10344,7 @@
         <v>681</v>
       </c>
       <c r="H94" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="I94" t="s">
         <v>695</v>
@@ -10457,10 +10457,10 @@
         <v>594</v>
       </c>
       <c r="G98" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="H98" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="I98" t="s">
         <v>691</v>
@@ -10468,115 +10468,115 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
         <v>99</v>
       </c>
-      <c r="B99" t="s">
-        <v>100</v>
-      </c>
       <c r="C99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D99" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E99" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F99" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G99" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="H99" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="I99" t="s">
-        <v>691</v>
+        <v>701</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
         <v>100</v>
       </c>
-      <c r="B100" t="s">
-        <v>101</v>
-      </c>
       <c r="C100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D100" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E100" t="s">
         <v>495</v>
       </c>
       <c r="F100" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G100" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="H100" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="I100" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
         <v>101</v>
       </c>
-      <c r="B101" t="s">
-        <v>102</v>
-      </c>
       <c r="C101" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D101" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E101" t="s">
         <v>495</v>
       </c>
       <c r="F101" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G101" t="s">
         <v>680</v>
       </c>
       <c r="H101" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="I101" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
         <v>102</v>
       </c>
-      <c r="B102" t="s">
-        <v>103</v>
-      </c>
       <c r="C102" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D102" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E102" t="s">
         <v>495</v>
       </c>
       <c r="F102" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G102" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="H102" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="I102" t="s">
         <v>692</v>
@@ -10584,115 +10584,115 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
         <v>103</v>
       </c>
-      <c r="B103" t="s">
-        <v>104</v>
-      </c>
       <c r="C103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D103" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E103" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F103" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G103" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H103" t="s">
-        <v>673</v>
+        <v>680</v>
       </c>
       <c r="I103" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
         <v>104</v>
       </c>
-      <c r="B104" t="s">
-        <v>105</v>
-      </c>
       <c r="C104" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D104" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E104" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="F104" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G104" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="H104" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="I104" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
         <v>105</v>
       </c>
-      <c r="B105" t="s">
-        <v>106</v>
-      </c>
       <c r="C105" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D105" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E105" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F105" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G105" t="s">
+        <v>685</v>
+      </c>
+      <c r="H105" t="s">
         <v>688</v>
       </c>
-      <c r="H105" t="s">
-        <v>684</v>
-      </c>
       <c r="I105" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
         <v>106</v>
       </c>
-      <c r="B106" t="s">
-        <v>107</v>
-      </c>
       <c r="C106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D106" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E106" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="F106" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G106" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="H106" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="I106" t="s">
         <v>691</v>
@@ -10700,25 +10700,25 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
         <v>107</v>
       </c>
-      <c r="B107" t="s">
-        <v>108</v>
-      </c>
       <c r="C107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D107" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E107" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F107" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G107" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H107" t="s">
         <v>684</v>
@@ -10729,25 +10729,25 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
         <v>108</v>
       </c>
-      <c r="B108" t="s">
-        <v>109</v>
-      </c>
       <c r="C108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D108" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E108" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F108" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="G108" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="H108" t="s">
         <v>684</v>
@@ -10758,28 +10758,28 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="1">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C109" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D109" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E109" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F109" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G109" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="H109" t="s">
-        <v>673</v>
+        <v>684</v>
       </c>
       <c r="I109" t="s">
         <v>691</v>
@@ -10787,28 +10787,28 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="1">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C110" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D110" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E110" t="s">
         <v>493</v>
       </c>
       <c r="F110" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="G110" t="s">
         <v>688</v>
       </c>
       <c r="H110" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="I110" t="s">
         <v>691</v>
@@ -10816,28 +10816,28 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="1">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D111" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E111" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="F111" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="G111" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="H111" t="s">
-        <v>688</v>
+        <v>676</v>
       </c>
       <c r="I111" t="s">
         <v>691</v>
@@ -10845,86 +10845,86 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="1">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C112" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D112" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E112" t="s">
         <v>493</v>
       </c>
       <c r="F112" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="G112" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="H112" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="I112" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="1">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C113" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D113" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="E113" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F113" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="G113" t="s">
         <v>687</v>
       </c>
       <c r="H113" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
       <c r="I113" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="1">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C114" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D114" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E114" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F114" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="G114" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
       <c r="H114" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="I114" t="s">
         <v>691</v>
@@ -10932,28 +10932,28 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="1">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C115" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="D115" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="E115" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F115" t="s">
-        <v>627</v>
+        <v>611</v>
       </c>
       <c r="G115" t="s">
         <v>686</v>
       </c>
       <c r="H115" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="I115" t="s">
         <v>691</v>
@@ -10961,57 +10961,57 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="1">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C116" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="D116" t="s">
-        <v>459</v>
+        <v>433</v>
       </c>
       <c r="E116" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F116" t="s">
-        <v>638</v>
+        <v>612</v>
       </c>
       <c r="G116" t="s">
         <v>686</v>
       </c>
       <c r="H116" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
       <c r="I116" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="1">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="C117" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="D117" t="s">
-        <v>461</v>
+        <v>434</v>
       </c>
       <c r="E117" t="s">
         <v>493</v>
       </c>
       <c r="F117" t="s">
-        <v>640</v>
+        <v>613</v>
       </c>
       <c r="G117" t="s">
         <v>686</v>
       </c>
       <c r="H117" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="I117" t="s">
         <v>691</v>
@@ -11019,28 +11019,28 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="1">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="C118" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="D118" t="s">
-        <v>472</v>
+        <v>436</v>
       </c>
       <c r="E118" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F118" t="s">
-        <v>651</v>
+        <v>615</v>
       </c>
       <c r="G118" t="s">
         <v>686</v>
       </c>
       <c r="H118" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="I118" t="s">
         <v>691</v>
@@ -11048,28 +11048,28 @@
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="1">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="C119" t="s">
-        <v>305</v>
+        <v>272</v>
       </c>
       <c r="D119" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
       <c r="E119" t="s">
         <v>494</v>
       </c>
       <c r="F119" t="s">
-        <v>655</v>
+        <v>617</v>
       </c>
       <c r="G119" t="s">
-        <v>673</v>
+        <v>686</v>
       </c>
       <c r="H119" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="I119" t="s">
         <v>691</v>
@@ -11077,28 +11077,28 @@
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="1">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="B120" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="C120" t="s">
-        <v>315</v>
+        <v>275</v>
       </c>
       <c r="D120" t="s">
-        <v>488</v>
+        <v>441</v>
       </c>
       <c r="E120" t="s">
         <v>494</v>
       </c>
       <c r="F120" t="s">
-        <v>667</v>
+        <v>620</v>
       </c>
       <c r="G120" t="s">
         <v>673</v>
       </c>
       <c r="H120" t="s">
-        <v>686</v>
+        <v>674</v>
       </c>
       <c r="I120" t="s">
         <v>691</v>

</xml_diff>